<commit_message>
if user does not exist, don't create
</commit_message>
<xml_diff>
--- a/zabbix_user_create.xlsx
+++ b/zabbix_user_create.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">user!$D:$D</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
   <si>
     <t>别名(alias)</t>
   </si>
@@ -28,13 +31,16 @@
     <t>用户类型(User type)</t>
   </si>
   <si>
-    <t>test</t>
+    <t>test14</t>
   </si>
   <si>
     <t>wangjinle</t>
   </si>
   <si>
     <t>guest,admin</t>
+  </si>
+  <si>
+    <t>super admin</t>
   </si>
 </sst>
 </file>
@@ -47,8 +53,16 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
-    <font>
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -200,12 +214,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -508,10 +528,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -520,142 +540,148 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1008,7 +1034,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1022,21 +1048,21 @@
     <col min="7" max="7" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:4">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1046,8 +1072,16 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:D$1048576">
+      <formula1>"user,admin,super admin"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
cell value which type is float should converts to string
</commit_message>
<xml_diff>
--- a/zabbix_user_create.xlsx
+++ b/zabbix_user_create.xlsx
@@ -1088,7 +1088,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="6"/>
@@ -1141,7 +1141,9 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2">
+        <v>15911111111</v>
+      </c>
       <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
@@ -1162,7 +1164,9 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <v>15911111112</v>
+      </c>
       <c r="G3" s="5" t="s">
         <v>18</v>
       </c>
@@ -1183,7 +1187,9 @@
       <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>15911111113</v>
+      </c>
       <c r="G4" s="5" t="s">
         <v>23</v>
       </c>

</xml_diff>